<commit_message>
[Cloudstitch Services] Project publish citipetacas/prueba
</commit_message>
<xml_diff>
--- a/API Spreadsheet.xlsx
+++ b/API Spreadsheet.xlsx
@@ -11,24 +11,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
-    <t>Name</t>
+    <t>Timestamp</t>
   </si>
   <si>
-    <t>Subject</t>
+    <t>Measurement</t>
   </si>
   <si>
-    <t>Message</t>
-  </si>
-  <si>
-    <t>Ted</t>
-  </si>
-  <si>
-    <t>Welcome to your API Spreadsheet!</t>
-  </si>
-  <si>
-    <t>Your Cloudstitch project exposes an endpoint that lets forms on your web site send data to this spreadsheet. Make sure you've created column names matching your form fields. For paid plans, we even auto-complete Stripe transactions and enable notifications (email, slack, sms, etc) based on these form posts!</t>
+    <t>101</t>
   </si>
 </sst>
 </file>
@@ -65,7 +56,7 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
@@ -109,9 +100,7 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C1" s="2"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
@@ -138,14 +127,12 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="C2" s="2"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>

</xml_diff>